<commit_message>
Included iteration2, QA tests and modified ERD, LDD
Included iteration2, QA tests and modified ERD, components of ERD,
Logical Database Description
</commit_message>
<xml_diff>
--- a/documentation/softdev/JFK_RTM.xlsx
+++ b/documentation/softdev/JFK_RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\softdev\apc-softdev-it111-02\documentation\softdev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\softdev2\apc-softdev-it111-02\documentation\softdev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>Project Name</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Easy to use interface</t>
   </si>
   <si>
-    <t>Has a login for admin</t>
-  </si>
-  <si>
-    <t>Admin has control on volunteer and subscribe module</t>
-  </si>
-  <si>
     <t>User can donate online</t>
   </si>
   <si>
@@ -110,21 +104,12 @@
     <t>User can cancel his/her donation</t>
   </si>
   <si>
-    <t>User can stop subscribing</t>
-  </si>
-  <si>
     <t>Admin can view records of volunteers</t>
   </si>
   <si>
     <t>Admin can view records of subscribers</t>
   </si>
   <si>
-    <t>Admin can approve requests</t>
-  </si>
-  <si>
-    <t>Admin can reject requests</t>
-  </si>
-  <si>
     <t>Admin can login</t>
   </si>
   <si>
@@ -140,9 +125,6 @@
     <t>R13</t>
   </si>
   <si>
-    <t>User can select many items in the shop</t>
-  </si>
-  <si>
     <t>R14</t>
   </si>
   <si>
@@ -176,12 +158,6 @@
     <t>Back End Login</t>
   </si>
   <si>
-    <t>Payment transaction is secured</t>
-  </si>
-  <si>
-    <t>Donation and Shopping Cart Module</t>
-  </si>
-  <si>
     <t>Shopping Cart Module</t>
   </si>
   <si>
@@ -191,47 +167,98 @@
     <t>Back End Subscriber Module</t>
   </si>
   <si>
-    <t>Volunteer Page</t>
-  </si>
-  <si>
     <t>Donation Page</t>
   </si>
   <si>
     <t>Donation Module</t>
   </si>
   <si>
-    <t>Back End module</t>
-  </si>
-  <si>
     <t>UITC_SeEm1</t>
   </si>
   <si>
-    <t>UITC_ReAp1</t>
-  </si>
-  <si>
-    <t>UITC_ApAp1</t>
-  </si>
-  <si>
     <t>UITC_Ev1</t>
+  </si>
+  <si>
+    <t>User can cancel his/her order</t>
+  </si>
+  <si>
+    <t>User can select buy products in the shop</t>
+  </si>
+  <si>
+    <t>Admin can email volunteers</t>
+  </si>
+  <si>
+    <t>Admin can email subscribers</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>Users can pay without PayPal account</t>
+  </si>
+  <si>
+    <t>Users can donate without PayPal account</t>
+  </si>
+  <si>
+    <t>UITC_SoCa1</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>Users can view all ordered items</t>
+  </si>
+  <si>
+    <t>Donation  Module</t>
+  </si>
+  <si>
+    <t>FTC_SoCa10</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>Online transactions are secured</t>
+  </si>
+  <si>
+    <t>Shopping Cart and Donation Module</t>
+  </si>
+  <si>
+    <t>FTC_SoCa12,</t>
+  </si>
+  <si>
+    <t>FTC_SoCa13,</t>
+  </si>
+  <si>
+    <t>FTC_SoCa16-</t>
+  </si>
+  <si>
+    <t>UITC_Do1</t>
+  </si>
+  <si>
+    <t>FTC_SoCa8,</t>
+  </si>
+  <si>
+    <t>FTC_SoCa9</t>
+  </si>
+  <si>
+    <t>FTC_SoCa23,</t>
+  </si>
+  <si>
+    <t>FTC_Do2-FTC_Do10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -256,7 +283,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,308 +631,386 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" t="s">
-        <v>48</v>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
+      <c r="G7" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
         <v>46</v>
       </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" t="s">
-        <v>53</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" t="s">
-        <v>51</v>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included revised RTM in the SQAP
Included revised RTM in the SQAP
</commit_message>
<xml_diff>
--- a/documentation/softdev/JFK_RTM.xlsx
+++ b/documentation/softdev/JFK_RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>Project Name</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Admin can view records of subscribers</t>
   </si>
   <si>
-    <t>Admin can login</t>
-  </si>
-  <si>
     <t>Any user can view the foundation's programs</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>Lowy Needed</t>
   </si>
   <si>
-    <t>R15</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>User Interface</t>
   </si>
   <si>
-    <t>Back End Login</t>
-  </si>
-  <si>
     <t>Shopping Cart Module</t>
   </si>
   <si>
@@ -191,33 +182,18 @@
     <t>Admin can email subscribers</t>
   </si>
   <si>
-    <t>R16</t>
-  </si>
-  <si>
     <t>Users can pay without PayPal account</t>
   </si>
   <si>
-    <t>Users can donate without PayPal account</t>
-  </si>
-  <si>
     <t>UITC_SoCa1</t>
   </si>
   <si>
-    <t>R17</t>
-  </si>
-  <si>
     <t>Users can view all ordered items</t>
   </si>
   <si>
-    <t>Donation  Module</t>
-  </si>
-  <si>
     <t>FTC_SoCa10</t>
   </si>
   <si>
-    <t>R18</t>
-  </si>
-  <si>
     <t>Online transactions are secured</t>
   </si>
   <si>
@@ -246,6 +222,36 @@
   </si>
   <si>
     <t>FTC_Do2-FTC_Do10</t>
+  </si>
+  <si>
+    <t>FTC_Do12</t>
+  </si>
+  <si>
+    <t>FTC_Do11</t>
+  </si>
+  <si>
+    <t>FTC_SoCa8</t>
+  </si>
+  <si>
+    <t>FTC_SoCa6,</t>
+  </si>
+  <si>
+    <t>FTC_SoCa7,</t>
+  </si>
+  <si>
+    <t>FTC_SoCa5</t>
+  </si>
+  <si>
+    <t>FTC_SoCa14</t>
+  </si>
+  <si>
+    <t>UITC_ReAp2</t>
+  </si>
+  <si>
+    <t>UITC_SeEm2</t>
+  </si>
+  <si>
+    <t>UITC_ReAp1</t>
   </si>
 </sst>
 </file>
@@ -566,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,24 +637,24 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
         <v>40</v>
       </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G7" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -656,104 +662,142 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="1"/>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -761,43 +805,45 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,213 +851,151 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="1"/>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="G24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="1" t="s">
-        <v>68</v>
+      <c r="G27" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G28" t="s">
-        <v>72</v>
-      </c>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G29" t="s">
-        <v>73</v>
-      </c>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>